<commit_message>
Passed: 125; Skipped: 98; Undo: 48
</commit_message>
<xml_diff>
--- a/dbi_test_cases.xlsx
+++ b/dbi_test_cases.xlsx
@@ -13,13 +13,13 @@
   </sheets>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="326">
   <si>
     <t>spec_getting_started</t>
   </si>
@@ -1016,6 +1016,18 @@
   </si>
   <si>
     <t xml:space="preserve">this test requires supporting NULL value. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>doesn't support bind</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1102,285 +1114,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Huang" refreshedDate="43082.594761111111" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="271">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Huang" refreshedDate="43082.749364930554" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="271">
   <cacheSource type="worksheet">
     <worksheetSource ref="B3:D274" sheet="工作表1"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="test-case" numFmtId="0">
-      <sharedItems count="271">
-        <s v="package_dependencies"/>
-        <s v="package_name"/>
-        <s v="inherits_from_driver"/>
-        <s v="constructor"/>
-        <s v="data_type_formals"/>
-        <s v="data_type_driver"/>
-        <s v="get_info_driver"/>
-        <s v="connect_formals"/>
-        <s v="can_connect"/>
-        <s v="disconnect_formals"/>
-        <s v="can_disconnect"/>
-        <s v="cannot_forget_disconnect"/>
-        <s v="disconnect_closed_connection"/>
-        <s v="disconnect_invalid_connection"/>
-        <s v="data_type_connection"/>
-        <s v="get_info_connection"/>
-        <s v="send_query_formals"/>
-        <s v="send_query_trivial"/>
-        <s v="send_query_closed_connection"/>
-        <s v="send_query_invalid_connection"/>
-        <s v="send_query_syntax_error"/>
-        <s v="send_query_non_string"/>
-        <s v="send_query_result_valid"/>
-        <s v="send_query_stale_warning"/>
-        <s v="send_query_only_one_result_set"/>
-        <s v="fetch_formals"/>
-        <s v="fetch_atomic"/>
-        <s v="fetch_one_row"/>
-        <s v="fetch_zero_rows"/>
-        <s v="fetch_closed"/>
-        <s v="fetch_n_bad"/>
-        <s v="fetch_n_good_after_bad"/>
-        <s v="fetch_no_return_value"/>
-        <s v="fetch_multi_row_single_column"/>
-        <s v="fetch_multi_row_multi_column"/>
-        <s v="fetch_n_progressive"/>
-        <s v="fetch_n_multi_row_inf"/>
-        <s v="fetch_n_more_rows"/>
-        <s v="fetch_n_zero_rows"/>
-        <s v="fetch_n_premature_close"/>
-        <s v="fetch_row_names"/>
-        <s v="clear_result_formals"/>
-        <s v="clear_result_return_query"/>
-        <s v="clear_result_return_statement"/>
-        <s v="cannot_clear_result_twice_query"/>
-        <s v="cannot_clear_result_twice_statement"/>
-        <s v="get_query_formals"/>
-        <s v="get_query_atomic"/>
-        <s v="get_query_one_row"/>
-        <s v="get_query_zero_rows"/>
-        <s v="get_query_closed_connection"/>
-        <s v="get_query_invalid_connection"/>
-        <s v="get_query_syntax_error"/>
-        <s v="get_query_non_string"/>
-        <s v="get_query_n_bad"/>
-        <s v="get_query_good_after_bad_n"/>
-        <s v="get_query_multi_row_single_column"/>
-        <s v="get_query_multi_row_multi_column"/>
-        <s v="get_query_n_multi_row_inf"/>
-        <s v="get_query_n_more_rows"/>
-        <s v="get_query_n_zero_rows"/>
-        <s v="get_query_n_incomplete"/>
-        <s v="get_query_row_names"/>
-        <s v="send_statement_formals"/>
-        <s v="send_statement_trivial"/>
-        <s v="send_statement_closed_connection"/>
-        <s v="send_statement_invalid_connection"/>
-        <s v="send_statement_syntax_error"/>
-        <s v="send_statement_non_string"/>
-        <s v="send_statement_result_valid"/>
-        <s v="send_statement_stale_warning"/>
-        <s v="send_statement_only_one_result_set"/>
-        <s v="execute_formals"/>
-        <s v="execute_atomic"/>
-        <s v="execute_closed_connection"/>
-        <s v="execute_invalid_connection"/>
-        <s v="execute_syntax_error"/>
-        <s v="execute_non_string"/>
-        <s v="data_type_create_table"/>
-        <s v="data_integer"/>
-        <s v="data_numeric"/>
-        <s v="data_logical"/>
-        <s v="data_character"/>
-        <s v="data_raw"/>
-        <s v="data_date"/>
-        <s v="data_date_current"/>
-        <s v="data_time"/>
-        <s v="data_time_current"/>
-        <s v="data_timestamp"/>
-        <s v="data_timestamp_current"/>
-        <s v="data_null"/>
-        <s v="data_date_typed"/>
-        <s v="data_date_current_typed"/>
-        <s v="data_timestamp_typed"/>
-        <s v="data_timestamp_current_typed"/>
-        <s v="data_64_bit_numeric"/>
-        <s v="data_64_bit_numeric_warning"/>
-        <s v="data_64_bit_lossless"/>
-        <s v="quote_string_formals"/>
-        <s v="quote_string_return"/>
-        <s v="quote_string_vectorized"/>
-        <s v="quote_string_double"/>
-        <s v="quote_string_roundtrip"/>
-        <s v="quote_string_na"/>
-        <s v="quote_string_na_is_null"/>
-        <s v="quote_identifier_formals"/>
-        <s v="quote_identifier_return"/>
-        <s v="quote_identifier_vectorized"/>
-        <s v="quote_identifier"/>
-        <s v="quote_identifier_string"/>
-        <s v="quote_identifier_special"/>
-        <s v="read_table_formals"/>
-        <s v="read_table"/>
-        <s v="read_table_missing"/>
-        <s v="read_table_empty"/>
-        <s v="read_table_row_names_false"/>
-        <s v="read_table_row_names_true_exists"/>
-        <s v="read_table_row_names_true_missing"/>
-        <s v="read_table_row_names_na_exists"/>
-        <s v="read_table_row_names_na_missing"/>
-        <s v="read_table_row_names_string_exists"/>
-        <s v="read_table_row_names_string_missing"/>
-        <s v="read_table_row_names_default"/>
-        <s v="read_table_check_names"/>
-        <s v="read_table_closed_connection"/>
-        <s v="read_table_invalid_connection"/>
-        <s v="read_table_error"/>
-        <s v="read_table_name"/>
-        <s v="write_table_formals"/>
-        <s v="write_table_return"/>
-        <s v="write_table_overwrite"/>
-        <s v="write_table_append_incompatible"/>
-        <s v="write_table_closed_connection"/>
-        <s v="write_table_invalid_connection"/>
-        <s v="write_table_error"/>
-        <s v="write_table_name"/>
-        <s v="overwrite_table"/>
-        <s v="overwrite_table_missing"/>
-        <s v="append_table"/>
-        <s v="append_table_new"/>
-        <s v="temporary_table"/>
-        <s v="table_visible_in_other_connection"/>
-        <s v="roundtrip_keywords"/>
-        <s v="roundtrip_quotes"/>
-        <s v="roundtrip_integer"/>
-        <s v="roundtrip_numeric"/>
-        <s v="roundtrip_logical"/>
-        <s v="roundtrip_null"/>
-        <s v="roundtrip_64_bit_numeric"/>
-        <s v="roundtrip_64_bit_character"/>
-        <s v="roundtrip_character"/>
-        <s v="roundtrip_character_native"/>
-        <s v="roundtrip_character_empty"/>
-        <s v="roundtrip_factor"/>
-        <s v="roundtrip_raw"/>
-        <s v="roundtrip_blob"/>
-        <s v="roundtrip_date"/>
-        <s v="roundtrip_time"/>
-        <s v="roundtrip_timestamp"/>
-        <s v="roundtrip_mixed"/>
-        <s v="roundtrip_field_types"/>
-        <s v="write_table_row_names_false"/>
-        <s v="write_table_row_names_true_exists"/>
-        <s v="write_table_row_names_true_missing"/>
-        <s v="write_table_row_names_na_exists"/>
-        <s v="write_table_row_names_na_missing"/>
-        <s v="write_table_row_names_string_exists"/>
-        <s v="write_table_row_names_string_missing"/>
-        <s v="list_tables_formals"/>
-        <s v="list_tables"/>
-        <s v="list_tables_closed_connection"/>
-        <s v="list_tables_invalid_connection"/>
-        <s v="exists_table_formals"/>
-        <s v="exists_table"/>
-        <s v="exists_table_closed_connection"/>
-        <s v="exists_table_invalid_connection"/>
-        <s v="exists_table_error"/>
-        <s v="exists_table_name"/>
-        <s v="exists_table_list"/>
-        <s v="remove_table_formals"/>
-        <s v="remove_table_return"/>
-        <s v="remove_table_missing"/>
-        <s v="remove_table_closed_connection"/>
-        <s v="remove_table_invalid_connection"/>
-        <s v="remove_table_error"/>
-        <s v="remove_table_list"/>
-        <s v="remove_table_other_con"/>
-        <s v="remove_table_temporary"/>
-        <s v="remove_table_name"/>
-        <s v="list_fields"/>
-        <s v="list_fields_row_names"/>
-        <s v="bind_formals"/>
-        <s v="bind_return_value"/>
-        <s v="bind_empty"/>
-        <s v="bind_too_many"/>
-        <s v="bind_not_enough"/>
-        <s v="bind_wrong_name"/>
-        <s v="bind_multi_row_unequal_length"/>
-        <s v="bind_named_param_unnamed_placeholders"/>
-        <s v="bind_named_param_empty_placeholders"/>
-        <s v="bind_named_param_na_placeholders"/>
-        <s v="bind_unnamed_param_named_placeholders"/>
-        <s v="bind_premature_clear"/>
-        <s v="bind_multi_row"/>
-        <s v="bind_multi_row_zero_length"/>
-        <s v="bind_multi_row_statement"/>
-        <s v="bind_repeated"/>
-        <s v="bind_repeated_untouched"/>
-        <s v="bind_integer"/>
-        <s v="bind_numeric"/>
-        <s v="bind_logical"/>
-        <s v="bind_null"/>
-        <s v="bind_character"/>
-        <s v="bind_factor"/>
-        <s v="bind_date"/>
-        <s v="bind_timestamp"/>
-        <s v="bind_timestamp_lt"/>
-        <s v="bind_raw"/>
-        <s v="bind_blob"/>
-        <s v="is_valid_formals"/>
-        <s v="is_valid_connection"/>
-        <s v="is_valid_stale_connection"/>
-        <s v="is_valid_result_query"/>
-        <s v="is_valid_result_statement"/>
-        <s v="has_completed_formals"/>
-        <s v="has_completed_query"/>
-        <s v="has_completed_statement"/>
-        <s v="has_completed_error"/>
-        <s v="has_completed_query_spec"/>
-        <s v="get_statement_formals"/>
-        <s v="get_statement_query"/>
-        <s v="get_statement_statement"/>
-        <s v="get_statement_error"/>
-        <s v="column_info"/>
-        <s v="get_row_count_formals"/>
-        <s v="row_count_query"/>
-        <s v="row_count_statement"/>
-        <s v="get_row_count_error"/>
-        <s v="get_rows_affected_formals"/>
-        <s v="rows_affected_statement"/>
-        <s v="rows_affected_query"/>
-        <s v="get_rows_affected_error"/>
-        <s v="get_info_result"/>
-        <s v="begin_formals"/>
-        <s v="commit_formals"/>
-        <s v="rollback_formals"/>
-        <s v="begin_commit_return_value"/>
-        <s v="begin_rollback_return_value"/>
-        <s v="begin_commit_closed"/>
-        <s v="begin_commit_invalid"/>
-        <s v="commit_without_begin"/>
-        <s v="rollback_without_begin"/>
-        <s v="begin_begin"/>
-        <s v="begin_commit"/>
-        <s v="begin_write_commit"/>
-        <s v="begin_rollback"/>
-        <s v="begin_write_rollback"/>
-        <s v="begin_write_disconnect"/>
-        <s v="with_transaction_formals"/>
-        <s v="with_transaction_return_value"/>
-        <s v="with_transaction_error_closed"/>
-        <s v="with_transaction_error_invalid"/>
-        <s v="with_transaction_error_nested"/>
-        <s v="with_transaction_success"/>
-        <s v="with_transaction_failure"/>
-        <s v="with_transaction_break"/>
-        <s v="with_transaction_side_effects"/>
-        <s v="compliance"/>
-        <s v="ellipsis"/>
-        <s v="simultaneous_connections"/>
-        <s v="stress_connections"/>
-      </sharedItems>
+      <sharedItems/>
     </cacheField>
     <cacheField name="status" numFmtId="0">
       <sharedItems containsBlank="1" count="3">
@@ -1390,7 +1130,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="comments" numFmtId="0">
-      <sharedItems containsBlank="1" count="16">
+      <sharedItems containsBlank="1" count="19">
         <m/>
         <s v="RMariaDB skips this"/>
         <s v="target is integer64, current is numeric"/>
@@ -1407,6 +1147,9 @@
         <s v="NULL is not supported"/>
         <s v="unlist(unname(rows)) not identical"/>
         <s v="dbGetQuery(con, &quot;SELECT \&quot;b\&quot; FROM (SELECT 1 AS \&quot;a\&quot;)&quot;) did not throw an error."/>
+        <s v="`actual` not identical to `expected`."/>
+        <s v="tweak disabled"/>
+        <s v="this test requires supporting NULL value. "/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -1421,1357 +1164,1357 @@
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="271">
   <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
+    <s v="package_dependencies"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="package_name"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="inherits_from_driver"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="constructor"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="data_type_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="data_type_driver"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_info_driver"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="connect_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="can_connect"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="disconnect_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="can_disconnect"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="cannot_forget_disconnect"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="disconnect_closed_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="disconnect_invalid_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="data_type_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_info_connection"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="send_query_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="send_query_trivial"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="send_query_closed_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="send_query_invalid_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="send_query_syntax_error"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="send_query_non_string"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="send_query_result_valid"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="send_query_stale_warning"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="send_query_only_one_result_set"/>
+    <x v="1"/>
     <x v="3"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
+  </r>
+  <r>
+    <s v="fetch_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="fetch_atomic"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="fetch_one_row"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="fetch_zero_rows"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="fetch_closed"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="fetch_n_bad"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="fetch_n_good_after_bad"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="fetch_no_return_value"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="fetch_multi_row_single_column"/>
+    <x v="1"/>
     <x v="4"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
+  </r>
+  <r>
+    <s v="fetch_multi_row_multi_column"/>
+    <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="fetch_n_progressive"/>
+    <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="fetch_n_multi_row_inf"/>
+    <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="fetch_n_more_rows"/>
+    <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="fetch_n_zero_rows"/>
+    <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="fetch_n_premature_close"/>
+    <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="fetch_row_names"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="clear_result_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="clear_result_return_query"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="clear_result_return_statement"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="cannot_clear_result_twice_query"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="cannot_clear_result_twice_statement"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_query_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_query_atomic"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="get_query_one_row"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="get_query_zero_rows"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_query_closed_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_query_invalid_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_query_syntax_error"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_query_non_string"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_query_n_bad"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_query_good_after_bad_n"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="get_query_multi_row_single_column"/>
+    <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="get_query_multi_row_multi_column"/>
+    <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="get_query_n_multi_row_inf"/>
+    <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="get_query_n_more_rows"/>
+    <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="get_query_n_zero_rows"/>
+    <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="get_query_n_incomplete"/>
+    <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="get_query_row_names"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="send_statement_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="send_statement_trivial"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="send_statement_closed_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="send_statement_invalid_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="send_statement_syntax_error"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="send_statement_non_string"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="send_statement_result_valid"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="send_statement_stale_warning"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="send_statement_only_one_result_set"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="execute_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="execute_atomic"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="execute_closed_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="execute_invalid_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="execute_syntax_error"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="execute_non_string"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="data_type_create_table"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="data_integer"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="data_numeric"/>
+    <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="data_logical"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="data_character"/>
+    <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="data_raw"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="data_date"/>
+    <x v="1"/>
     <x v="5"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
+  </r>
+  <r>
+    <s v="data_date_current"/>
+    <x v="1"/>
     <x v="6"/>
-    <x v="1"/>
-    <x v="1"/>
-  </r>
-  <r>
+  </r>
+  <r>
+    <s v="data_time"/>
+    <x v="1"/>
     <x v="7"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
+  </r>
+  <r>
+    <s v="data_time_current"/>
+    <x v="1"/>
     <x v="8"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
+  </r>
+  <r>
+    <s v="data_timestamp"/>
+    <x v="1"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <s v="data_timestamp_current"/>
+    <x v="1"/>
     <x v="9"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
+  </r>
+  <r>
+    <s v="data_null"/>
+    <x v="1"/>
     <x v="10"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
+  </r>
+  <r>
+    <s v="data_date_typed"/>
+    <x v="1"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="data_date_current_typed"/>
+    <x v="1"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="data_timestamp_typed"/>
+    <x v="1"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <s v="data_timestamp_current_typed"/>
+    <x v="1"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <s v="data_64_bit_numeric"/>
+    <x v="1"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <s v="data_64_bit_numeric_warning"/>
+    <x v="1"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <s v="data_64_bit_lossless"/>
+    <x v="1"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <s v="quote_string_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="quote_string_return"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="quote_string_vectorized"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="quote_string_double"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="quote_string_roundtrip"/>
+    <x v="1"/>
     <x v="11"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
+  </r>
+  <r>
+    <s v="quote_string_na"/>
+    <x v="1"/>
     <x v="12"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
+  </r>
+  <r>
+    <s v="quote_string_na_is_null"/>
+    <x v="1"/>
     <x v="13"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
+  </r>
+  <r>
+    <s v="quote_identifier_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="quote_identifier_return"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="quote_identifier_vectorized"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="quote_identifier"/>
+    <x v="1"/>
     <x v="14"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
+  </r>
+  <r>
+    <s v="quote_identifier_string"/>
+    <x v="1"/>
     <x v="15"/>
-    <x v="1"/>
-    <x v="1"/>
-  </r>
-  <r>
+  </r>
+  <r>
+    <s v="quote_identifier_special"/>
+    <x v="1"/>
+    <x v="14"/>
+  </r>
+  <r>
+    <s v="read_table_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_missing"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_empty"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_row_names_false"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_row_names_true_exists"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_row_names_true_missing"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_row_names_na_exists"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_row_names_na_missing"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_row_names_string_exists"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_row_names_string_missing"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_row_names_default"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_check_names"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_closed_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_invalid_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_error"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_name"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="write_table_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="write_table_return"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="write_table_overwrite"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="write_table_append_incompatible"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="write_table_closed_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="write_table_invalid_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="write_table_error"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="write_table_name"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="overwrite_table"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="overwrite_table_missing"/>
+    <x v="1"/>
     <x v="16"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
+  </r>
+  <r>
+    <s v="append_table"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="append_table_new"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="temporary_table"/>
+    <x v="0"/>
     <x v="17"/>
-    <x v="1"/>
-    <x v="2"/>
-  </r>
-  <r>
+  </r>
+  <r>
+    <s v="table_visible_in_other_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="roundtrip_keywords"/>
+    <x v="1"/>
     <x v="18"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="19"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="20"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="21"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="22"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="23"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="24"/>
-    <x v="1"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="25"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="26"/>
-    <x v="1"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="27"/>
-    <x v="1"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="28"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="29"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="30"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="31"/>
-    <x v="1"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="32"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="33"/>
-    <x v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="34"/>
-    <x v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="35"/>
-    <x v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="36"/>
-    <x v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="37"/>
-    <x v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="38"/>
-    <x v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="39"/>
-    <x v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="40"/>
-    <x v="1"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="41"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="42"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="43"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="44"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="45"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="46"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="47"/>
-    <x v="1"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="48"/>
-    <x v="1"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="49"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="50"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="51"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="52"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="53"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="54"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="55"/>
-    <x v="1"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="56"/>
-    <x v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="57"/>
-    <x v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="58"/>
-    <x v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="59"/>
-    <x v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="60"/>
-    <x v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="61"/>
-    <x v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="62"/>
-    <x v="1"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="63"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="64"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="65"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="66"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="67"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="68"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="69"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="70"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="71"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="72"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="73"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="74"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="75"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="76"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="77"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="78"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="79"/>
-    <x v="1"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="80"/>
-    <x v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="81"/>
-    <x v="1"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="82"/>
-    <x v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="83"/>
-    <x v="1"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="84"/>
-    <x v="1"/>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="85"/>
-    <x v="1"/>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="86"/>
-    <x v="1"/>
-    <x v="7"/>
-  </r>
-  <r>
-    <x v="87"/>
-    <x v="1"/>
-    <x v="8"/>
-  </r>
-  <r>
-    <x v="88"/>
-    <x v="1"/>
-    <x v="7"/>
-  </r>
-  <r>
-    <x v="89"/>
-    <x v="1"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="90"/>
-    <x v="1"/>
-    <x v="10"/>
-  </r>
-  <r>
-    <x v="91"/>
-    <x v="1"/>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="92"/>
-    <x v="1"/>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="93"/>
-    <x v="1"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="94"/>
-    <x v="1"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="95"/>
-    <x v="1"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="96"/>
-    <x v="1"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="97"/>
-    <x v="1"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="98"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="99"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="100"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="101"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="102"/>
-    <x v="1"/>
-    <x v="11"/>
-  </r>
-  <r>
-    <x v="103"/>
-    <x v="1"/>
-    <x v="12"/>
-  </r>
-  <r>
-    <x v="104"/>
-    <x v="1"/>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="105"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="106"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="107"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="108"/>
-    <x v="1"/>
-    <x v="14"/>
-  </r>
-  <r>
-    <x v="109"/>
-    <x v="1"/>
-    <x v="15"/>
-  </r>
-  <r>
-    <x v="110"/>
-    <x v="1"/>
-    <x v="14"/>
-  </r>
-  <r>
-    <x v="111"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="112"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="113"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="114"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="115"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="116"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="117"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="118"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="119"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="120"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="121"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="122"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="123"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="124"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="125"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="126"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="127"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="128"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="129"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="130"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="131"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="132"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="133"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="134"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="135"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="136"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="137"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="138"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="139"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="140"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="141"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="142"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="143"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="144"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="145"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="146"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="147"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="148"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="149"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="150"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="151"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="152"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="153"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="154"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="155"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="156"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="157"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="158"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="159"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="160"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="161"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="162"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="163"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="164"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="165"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="166"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="167"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="168"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="169"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="170"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="171"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="172"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="173"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="174"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="175"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="176"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="177"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="178"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="179"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="180"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="181"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="182"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="183"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="184"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="185"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="186"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="187"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="188"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="189"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="190"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="191"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="192"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="193"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="194"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="195"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="196"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="197"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="198"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="199"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="200"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="201"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="202"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="203"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="204"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="205"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="206"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="207"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="208"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="209"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="210"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="211"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="212"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="213"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="214"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="215"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="216"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="217"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="218"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="219"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="220"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="221"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="222"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="223"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="224"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="225"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="226"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="227"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="228"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="229"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="230"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="231"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="232"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="233"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="234"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="235"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="236"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="237"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="238"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="239"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="240"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="241"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="242"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="243"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="244"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="245"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="246"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="247"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="248"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="249"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="250"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="251"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="252"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="253"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="254"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="255"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="256"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="257"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="258"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="259"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="260"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="261"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="262"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="263"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="264"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="265"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="266"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="267"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="268"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="269"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="270"/>
+  </r>
+  <r>
+    <s v="roundtrip_quotes"/>
+    <x v="1"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <s v="roundtrip_integer"/>
+    <x v="1"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <s v="roundtrip_numeric"/>
+    <x v="1"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <s v="roundtrip_logical"/>
+    <x v="1"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <s v="roundtrip_null"/>
+    <x v="1"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <s v="roundtrip_64_bit_numeric"/>
+    <x v="1"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <s v="roundtrip_64_bit_character"/>
+    <x v="1"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <s v="roundtrip_character"/>
+    <x v="1"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <s v="roundtrip_character_native"/>
+    <x v="1"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <s v="roundtrip_character_empty"/>
+    <x v="1"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <s v="roundtrip_factor"/>
+    <x v="1"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <s v="roundtrip_raw"/>
+    <x v="1"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <s v="roundtrip_blob"/>
+    <x v="1"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <s v="roundtrip_date"/>
+    <x v="1"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <s v="roundtrip_time"/>
+    <x v="1"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <s v="roundtrip_timestamp"/>
+    <x v="1"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <s v="roundtrip_mixed"/>
+    <x v="1"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <s v="roundtrip_field_types"/>
+    <x v="1"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <s v="write_table_row_names_false"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="write_table_row_names_true_exists"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="write_table_row_names_true_missing"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="write_table_row_names_na_exists"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="write_table_row_names_na_missing"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="write_table_row_names_string_exists"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="write_table_row_names_string_missing"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="list_tables_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="list_tables"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="list_tables_closed_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="list_tables_invalid_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="exists_table_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="exists_table"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="exists_table_closed_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="exists_table_invalid_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="exists_table_error"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="exists_table_name"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="exists_table_list"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="remove_table_formals"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="remove_table_return"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="remove_table_missing"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="remove_table_closed_connection"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="remove_table_invalid_connection"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="remove_table_error"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="remove_table_list"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="remove_table_other_con"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="remove_table_temporary"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="remove_table_name"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="list_fields"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="list_fields_row_names"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_formals"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_return_value"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_empty"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_too_many"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_not_enough"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_wrong_name"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_multi_row_unequal_length"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_named_param_unnamed_placeholders"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_named_param_empty_placeholders"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_named_param_na_placeholders"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_unnamed_param_named_placeholders"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_premature_clear"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_multi_row"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_multi_row_zero_length"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_multi_row_statement"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_repeated"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_repeated_untouched"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_integer"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_numeric"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_logical"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_null"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_character"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_factor"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_date"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_timestamp"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_timestamp_lt"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_raw"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_blob"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="is_valid_formals"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="is_valid_connection"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="is_valid_stale_connection"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="is_valid_result_query"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="is_valid_result_statement"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="has_completed_formals"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="has_completed_query"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="has_completed_statement"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="has_completed_error"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="has_completed_query_spec"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_statement_formals"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_statement_query"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_statement_statement"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_statement_error"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="column_info"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_row_count_formals"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="row_count_query"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="row_count_statement"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_row_count_error"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_rows_affected_formals"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="rows_affected_statement"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="rows_affected_query"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_rows_affected_error"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_info_result"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="begin_formals"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="commit_formals"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="rollback_formals"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="begin_commit_return_value"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="begin_rollback_return_value"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="begin_commit_closed"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="begin_commit_invalid"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="commit_without_begin"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="rollback_without_begin"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="begin_begin"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="begin_commit"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="begin_write_commit"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="begin_rollback"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="begin_write_rollback"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="begin_write_disconnect"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="with_transaction_formals"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="with_transaction_return_value"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="with_transaction_error_closed"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="with_transaction_error_invalid"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="with_transaction_error_nested"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="with_transaction_success"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="with_transaction_failure"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="with_transaction_break"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="with_transaction_side_effects"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="compliance"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="ellipsis"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="simultaneous_connections"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="stress_connections"/>
     <x v="2"/>
     <x v="0"/>
   </r>
@@ -2779,285 +2522,10 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="樞紐分析表1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="數值" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="樞紐分析表1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="數值" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
-    <pivotField dataField="1" showAll="0">
-      <items count="272">
-        <item x="138"/>
-        <item x="139"/>
-        <item x="252"/>
-        <item x="253"/>
-        <item x="248"/>
-        <item x="249"/>
-        <item x="246"/>
-        <item x="243"/>
-        <item x="255"/>
-        <item x="247"/>
-        <item x="254"/>
-        <item x="257"/>
-        <item x="256"/>
-        <item x="218"/>
-        <item x="212"/>
-        <item x="214"/>
-        <item x="193"/>
-        <item x="213"/>
-        <item x="191"/>
-        <item x="208"/>
-        <item x="210"/>
-        <item x="203"/>
-        <item x="205"/>
-        <item x="197"/>
-        <item x="204"/>
-        <item x="199"/>
-        <item x="200"/>
-        <item x="198"/>
-        <item x="195"/>
-        <item x="211"/>
-        <item x="209"/>
-        <item x="202"/>
-        <item x="217"/>
-        <item x="206"/>
-        <item x="207"/>
-        <item x="192"/>
-        <item x="215"/>
-        <item x="216"/>
-        <item x="194"/>
-        <item x="201"/>
-        <item x="196"/>
-        <item x="8"/>
-        <item x="10"/>
-        <item x="44"/>
-        <item x="45"/>
-        <item x="11"/>
-        <item x="41"/>
-        <item x="42"/>
-        <item x="43"/>
-        <item x="233"/>
-        <item x="244"/>
-        <item x="250"/>
-        <item x="267"/>
-        <item x="7"/>
-        <item x="3"/>
-        <item x="97"/>
-        <item x="95"/>
-        <item x="96"/>
-        <item x="82"/>
-        <item x="84"/>
-        <item x="85"/>
-        <item x="92"/>
-        <item x="91"/>
-        <item x="79"/>
-        <item x="81"/>
-        <item x="90"/>
-        <item x="80"/>
-        <item x="83"/>
-        <item x="86"/>
-        <item x="87"/>
-        <item x="88"/>
-        <item x="89"/>
-        <item x="94"/>
-        <item x="93"/>
-        <item x="14"/>
-        <item x="78"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="12"/>
-        <item x="9"/>
-        <item x="13"/>
-        <item x="268"/>
-        <item x="73"/>
-        <item x="74"/>
-        <item x="72"/>
-        <item x="75"/>
-        <item x="77"/>
-        <item x="76"/>
-        <item x="173"/>
-        <item x="174"/>
-        <item x="176"/>
-        <item x="172"/>
-        <item x="175"/>
-        <item x="178"/>
-        <item x="177"/>
-        <item x="26"/>
-        <item x="29"/>
-        <item x="25"/>
-        <item x="34"/>
-        <item x="33"/>
-        <item x="30"/>
-        <item x="31"/>
-        <item x="37"/>
-        <item x="36"/>
-        <item x="39"/>
-        <item x="35"/>
-        <item x="38"/>
-        <item x="32"/>
-        <item x="27"/>
-        <item x="40"/>
-        <item x="28"/>
-        <item x="15"/>
-        <item x="6"/>
-        <item x="242"/>
-        <item x="47"/>
-        <item x="50"/>
-        <item x="46"/>
-        <item x="55"/>
-        <item x="51"/>
-        <item x="57"/>
-        <item x="56"/>
-        <item x="54"/>
-        <item x="61"/>
-        <item x="59"/>
-        <item x="58"/>
-        <item x="60"/>
-        <item x="53"/>
-        <item x="48"/>
-        <item x="62"/>
-        <item x="52"/>
-        <item x="49"/>
-        <item x="237"/>
-        <item x="234"/>
-        <item x="241"/>
-        <item x="238"/>
-        <item x="232"/>
-        <item x="229"/>
-        <item x="230"/>
-        <item x="231"/>
-        <item x="227"/>
-        <item x="224"/>
-        <item x="225"/>
-        <item x="228"/>
-        <item x="226"/>
-        <item x="2"/>
-        <item x="220"/>
-        <item x="219"/>
-        <item x="222"/>
-        <item x="223"/>
-        <item x="221"/>
-        <item x="189"/>
-        <item x="190"/>
-        <item x="169"/>
-        <item x="170"/>
-        <item x="168"/>
-        <item x="171"/>
-        <item x="136"/>
-        <item x="137"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="108"/>
-        <item x="105"/>
-        <item x="106"/>
-        <item x="110"/>
-        <item x="109"/>
-        <item x="107"/>
-        <item x="101"/>
-        <item x="98"/>
-        <item x="103"/>
-        <item x="104"/>
-        <item x="99"/>
-        <item x="102"/>
-        <item x="100"/>
-        <item x="112"/>
-        <item x="123"/>
-        <item x="124"/>
-        <item x="114"/>
-        <item x="126"/>
-        <item x="111"/>
-        <item x="125"/>
-        <item x="113"/>
-        <item x="127"/>
-        <item x="122"/>
-        <item x="115"/>
-        <item x="118"/>
-        <item x="119"/>
-        <item x="120"/>
-        <item x="121"/>
-        <item x="116"/>
-        <item x="117"/>
-        <item x="182"/>
-        <item x="184"/>
-        <item x="179"/>
-        <item x="183"/>
-        <item x="185"/>
-        <item x="181"/>
-        <item x="188"/>
-        <item x="186"/>
-        <item x="180"/>
-        <item x="187"/>
-        <item x="245"/>
-        <item x="251"/>
-        <item x="149"/>
-        <item x="148"/>
-        <item x="155"/>
-        <item x="150"/>
-        <item x="152"/>
-        <item x="151"/>
-        <item x="156"/>
-        <item x="153"/>
-        <item x="160"/>
-        <item x="144"/>
-        <item x="142"/>
-        <item x="146"/>
-        <item x="159"/>
-        <item x="147"/>
-        <item x="145"/>
-        <item x="143"/>
-        <item x="154"/>
-        <item x="157"/>
-        <item x="158"/>
-        <item x="235"/>
-        <item x="236"/>
-        <item x="240"/>
-        <item x="239"/>
-        <item x="18"/>
-        <item x="16"/>
-        <item x="19"/>
-        <item x="21"/>
-        <item x="24"/>
-        <item x="22"/>
-        <item x="23"/>
-        <item x="20"/>
-        <item x="17"/>
-        <item x="65"/>
-        <item x="63"/>
-        <item x="66"/>
-        <item x="68"/>
-        <item x="71"/>
-        <item x="69"/>
-        <item x="70"/>
-        <item x="67"/>
-        <item x="64"/>
-        <item x="269"/>
-        <item x="270"/>
-        <item x="141"/>
-        <item x="140"/>
-        <item x="265"/>
-        <item x="260"/>
-        <item x="261"/>
-        <item x="262"/>
-        <item x="264"/>
-        <item x="258"/>
-        <item x="259"/>
-        <item x="266"/>
-        <item x="263"/>
-        <item x="131"/>
-        <item x="132"/>
-        <item x="134"/>
-        <item x="128"/>
-        <item x="133"/>
-        <item x="135"/>
-        <item x="130"/>
-        <item x="129"/>
-        <item x="161"/>
-        <item x="164"/>
-        <item x="165"/>
-        <item x="166"/>
-        <item x="167"/>
-        <item x="162"/>
-        <item x="163"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="4">
         <item sd="0" x="0"/>
@@ -3067,7 +2535,7 @@
       </items>
     </pivotField>
     <pivotField axis="axisRow" showAll="0">
-      <items count="17">
+      <items count="20">
         <item x="15"/>
         <item x="3"/>
         <item x="13"/>
@@ -3084,6 +2552,9 @@
         <item x="11"/>
         <item x="10"/>
         <item x="0"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -3410,8 +2881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
-      <selection activeCell="C184" sqref="C184"/>
+    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
+      <selection activeCell="C227" sqref="C227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -5434,6 +4905,9 @@
       <c r="B183" s="1" t="s">
         <v>186</v>
       </c>
+      <c r="C183" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="D183" s="1"/>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -5441,6 +4915,9 @@
       <c r="B184" s="1" t="s">
         <v>187</v>
       </c>
+      <c r="C184" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="D184" s="1"/>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -5448,6 +4925,9 @@
       <c r="B185" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="C185" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="D185" s="1"/>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -5455,6 +4935,9 @@
       <c r="B186" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="C186" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="D186" s="1"/>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -5462,6 +4945,9 @@
       <c r="B187" s="1" t="s">
         <v>190</v>
       </c>
+      <c r="C187" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="D187" s="1"/>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -5469,6 +4955,9 @@
       <c r="B188" s="1" t="s">
         <v>191</v>
       </c>
+      <c r="C188" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="D188" s="1"/>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -5476,6 +4965,9 @@
       <c r="B189" s="1" t="s">
         <v>192</v>
       </c>
+      <c r="C189" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="D189" s="1"/>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -5483,6 +4975,9 @@
       <c r="B190" s="1" t="s">
         <v>193</v>
       </c>
+      <c r="C190" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="D190" s="1"/>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -5490,6 +4985,9 @@
       <c r="B191" s="1" t="s">
         <v>194</v>
       </c>
+      <c r="C191" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="D191" s="1"/>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -5497,6 +4995,9 @@
       <c r="B192" s="1" t="s">
         <v>195</v>
       </c>
+      <c r="C192" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="D192" s="1"/>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -5504,6 +5005,9 @@
       <c r="B193" s="1" t="s">
         <v>196</v>
       </c>
+      <c r="C193" s="1" t="s">
+        <v>323</v>
+      </c>
       <c r="D193" s="1"/>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -5511,6 +5015,9 @@
       <c r="B194" s="1" t="s">
         <v>197</v>
       </c>
+      <c r="C194" s="1" t="s">
+        <v>323</v>
+      </c>
       <c r="D194" s="1"/>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -5520,202 +5027,345 @@
       <c r="B195" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="D195" s="1"/>
+      <c r="C195" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
       <c r="B196" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="D196" s="1"/>
+      <c r="C196" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
       <c r="B197" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="D197" s="1"/>
+      <c r="C197" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D197" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
       <c r="B198" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D198" s="1"/>
+      <c r="C198" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
       <c r="B199" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D199" s="1"/>
+      <c r="C199" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
       <c r="B200" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="D200" s="1"/>
+      <c r="C200" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="1"/>
       <c r="B201" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D201" s="1"/>
+      <c r="C201" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="1"/>
       <c r="B202" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="D202" s="1"/>
+      <c r="C202" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="1"/>
       <c r="B203" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="D203" s="1"/>
+      <c r="C203" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="1"/>
       <c r="B204" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="D204" s="1"/>
+      <c r="C204" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D204" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="1"/>
       <c r="B205" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="D205" s="1"/>
+      <c r="C205" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D205" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="1"/>
       <c r="B206" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="D206" s="1"/>
+      <c r="C206" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D206" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="1"/>
       <c r="B207" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="D207" s="1"/>
+      <c r="C207" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D207" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="1"/>
       <c r="B208" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="D208" s="1"/>
+      <c r="C208" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D208" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="1"/>
       <c r="B209" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="D209" s="1"/>
+      <c r="C209" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="1"/>
       <c r="B210" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="D210" s="1"/>
+      <c r="C210" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="1"/>
       <c r="B211" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="D211" s="1"/>
+      <c r="C211" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="1"/>
       <c r="B212" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="D212" s="1"/>
+      <c r="C212" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D212" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="1"/>
       <c r="B213" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="D213" s="1"/>
+      <c r="C213" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="1"/>
       <c r="B214" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="D214" s="1"/>
+      <c r="C214" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="1"/>
       <c r="B215" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="D215" s="1"/>
+      <c r="C215" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D215" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="1"/>
       <c r="B216" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="D216" s="1"/>
+      <c r="C216" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="1"/>
       <c r="B217" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D217" s="1"/>
+      <c r="C217" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="1"/>
       <c r="B218" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D218" s="1"/>
+      <c r="C218" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="1"/>
       <c r="B219" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="D219" s="1"/>
+      <c r="C219" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D219" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="1"/>
       <c r="B220" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="D220" s="1"/>
+      <c r="C220" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="1"/>
       <c r="B221" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D221" s="1"/>
+      <c r="C221" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="1"/>
       <c r="B222" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D222" s="1"/>
+      <c r="C222" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="1"/>
       <c r="B223" s="1" t="s">
         <v>226</v>
       </c>
+      <c r="C223" s="1" t="s">
+        <v>323</v>
+      </c>
       <c r="D223" s="1"/>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -5723,6 +5373,9 @@
       <c r="B224" s="1" t="s">
         <v>227</v>
       </c>
+      <c r="C224" s="1" t="s">
+        <v>323</v>
+      </c>
       <c r="D224" s="1"/>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
@@ -5730,12 +5383,18 @@
       <c r="B225" s="1" t="s">
         <v>228</v>
       </c>
+      <c r="C225" s="1" t="s">
+        <v>323</v>
+      </c>
       <c r="D225" s="1"/>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="1"/>
       <c r="B226" s="1" t="s">
         <v>229</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>323</v>
       </c>
       <c r="D226" s="1"/>
     </row>
@@ -6093,7 +5752,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -6115,7 +5774,7 @@
         <v>308</v>
       </c>
       <c r="B2" s="5">
-        <v>86</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -6123,7 +5782,7 @@
         <v>303</v>
       </c>
       <c r="B3" s="5">
-        <v>50</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -6131,7 +5790,7 @@
         <v>318</v>
       </c>
       <c r="B4" s="5">
-        <v>135</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Replace backend driver with RMySQL
Tested cases:
DBItest::test_getting_started()
DBItest::test_driver(skip=test_driver_skip)
DBItest::test_connection(skip=test_connection_skip)
DBItest::test_result(skip=test_result_skip)
</commit_message>
<xml_diff>
--- a/dbi_test_cases.xlsx
+++ b/dbi_test_cases.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cheng-Ching\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="26955" windowHeight="12795"/>
+    <workbookView xWindow="1470" yWindow="30" windowWidth="26955" windowHeight="12795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="328">
   <si>
     <t>spec_getting_started</t>
   </si>
@@ -1029,12 +1034,18 @@
   <si>
     <t>doesn't support bind</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>internal error in RS_DBI_getConnection: corrupt connection handle</t>
+  </si>
+  <si>
+    <t>gc() showed 0 warnings</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1109,12 +1120,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Huang" refreshedDate="43082.749364930554" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="271">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Huang" refreshedDate="43083.759305439817" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="271" xr:uid="{00000000-000A-0000-FFFF-FFFF08000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="B3:D274" sheet="工作表1"/>
   </cacheSource>
@@ -1130,7 +1144,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="comments" numFmtId="0">
-      <sharedItems containsBlank="1" count="19">
+      <sharedItems containsBlank="1" count="20">
         <m/>
         <s v="RMariaDB skips this"/>
         <s v="target is integer64, current is numeric"/>
@@ -1150,6 +1164,7 @@
         <s v="`actual` not identical to `expected`."/>
         <s v="tweak disabled"/>
         <s v="this test requires supporting NULL value. "/>
+        <s v="doesn't support bind"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -2060,222 +2075,222 @@
   </r>
   <r>
     <s v="remove_table_formals"/>
-    <x v="2"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <s v="remove_table_return"/>
-    <x v="2"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <s v="remove_table_missing"/>
-    <x v="2"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <s v="remove_table_closed_connection"/>
-    <x v="2"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <s v="remove_table_invalid_connection"/>
-    <x v="2"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <s v="remove_table_error"/>
-    <x v="2"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <s v="remove_table_list"/>
-    <x v="2"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <s v="remove_table_other_con"/>
-    <x v="2"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <s v="remove_table_temporary"/>
-    <x v="2"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <s v="remove_table_name"/>
-    <x v="2"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <s v="list_fields"/>
-    <x v="2"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <s v="list_fields_row_names"/>
-    <x v="2"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <s v="bind_formals"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_return_value"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_empty"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_too_many"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_not_enough"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_wrong_name"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_multi_row_unequal_length"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_named_param_unnamed_placeholders"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_named_param_empty_placeholders"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_named_param_na_placeholders"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_unnamed_param_named_placeholders"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_premature_clear"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_multi_row"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_multi_row_zero_length"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_multi_row_statement"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_repeated"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_repeated_untouched"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_integer"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_numeric"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_logical"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_null"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_character"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_factor"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_date"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_timestamp"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_timestamp_lt"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_raw"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="bind_blob"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="19"/>
   </r>
   <r>
     <s v="is_valid_formals"/>
-    <x v="2"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <s v="is_valid_connection"/>
-    <x v="2"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <s v="is_valid_stale_connection"/>
-    <x v="2"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <s v="is_valid_result_query"/>
-    <x v="2"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
@@ -2522,7 +2537,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="樞紐分析表1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="數值" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="樞紐分析表1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="數值" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" showAll="0"/>
@@ -2535,7 +2550,7 @@
       </items>
     </pivotField>
     <pivotField axis="axisRow" showAll="0">
-      <items count="20">
+      <items count="21">
         <item x="15"/>
         <item x="3"/>
         <item x="13"/>
@@ -2555,6 +2570,7 @@
         <item x="16"/>
         <item x="17"/>
         <item x="18"/>
+        <item x="19"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2587,6 +2603,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
     </ext>
   </extLst>
 </pivotTableDefinition>
@@ -2635,7 +2654,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2668,9 +2687,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2703,6 +2739,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2878,11 +2931,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
-      <selection activeCell="C227" sqref="C227"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3043,9 +3096,11 @@
         <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D15" s="1"/>
+        <v>288</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
@@ -3063,9 +3118,11 @@
         <v>18</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D17" s="1"/>
+        <v>288</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
@@ -3107,11 +3164,9 @@
         <v>23</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>290</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="D21" s="1"/>
       <c r="E21" s="2">
         <v>43081</v>
       </c>
@@ -3132,9 +3187,11 @@
         <v>25</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="D23" s="1"/>
+        <v>288</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
@@ -3507,9 +3564,11 @@
         <v>57</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="D55" s="1"/>
+        <v>288</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
@@ -3673,9 +3732,11 @@
         <v>72</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D70" s="1"/>
+        <v>288</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
@@ -3763,9 +3824,11 @@
         <v>81</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D79" s="1"/>
+        <v>288</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
@@ -5748,11 +5811,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -5774,7 +5837,7 @@
         <v>308</v>
       </c>
       <c r="B2" s="5">
-        <v>109</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5782,7 +5845,7 @@
         <v>303</v>
       </c>
       <c r="B3" s="5">
-        <v>70</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -5790,7 +5853,7 @@
         <v>318</v>
       </c>
       <c r="B4" s="5">
-        <v>92</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -5808,7 +5871,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Done. Passed: 132; Skipped: 139
</commit_message>
<xml_diff>
--- a/dbi_test_cases.xlsx
+++ b/dbi_test_cases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="30" windowWidth="26955" windowHeight="12795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3690" yWindow="30" windowWidth="26955" windowHeight="12795" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,13 @@
   </sheets>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="12" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="344">
   <si>
     <t>spec_getting_started</t>
   </si>
@@ -1000,9 +1000,6 @@
     <t>總計</t>
   </si>
   <si>
-    <t>(空白)</t>
-  </si>
-  <si>
     <t>計數 - test-case</t>
   </si>
   <si>
@@ -1036,6 +1033,65 @@
   </si>
   <si>
     <t>Objects equal but not identical</t>
+  </si>
+  <si>
+    <t>p</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>server hang</t>
+  </si>
+  <si>
+    <t>bo returned 0 rows effected</t>
+  </si>
+  <si>
+    <t>bo returned 0 rows effected</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>affected shows -1</t>
+  </si>
+  <si>
+    <t>affected shows -1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rstats-db/DBI#55</t>
+  </si>
+  <si>
+    <t>rstats-db/RSQLite#117</t>
+  </si>
+  <si>
+    <t>NULL is not supported</t>
+  </si>
+  <si>
+    <t>Object doesn't exist: function 'date'</t>
+  </si>
+  <si>
+    <t>RMariaDB skips this</t>
+  </si>
+  <si>
+    <t>unlist(unname(rows)) not identical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this test requires supporting NULL value. </t>
+  </si>
+  <si>
+    <t>doesn't support bind</t>
+  </si>
+  <si>
+    <t>doesn't support transaction</t>
+  </si>
+  <si>
+    <t>doesn't support transaction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cannot allocate a new connection: 16 connections already opened</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1143,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1105,6 +1161,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1124,7 +1183,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Huang" refreshedDate="43083.759305439817" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="271" xr:uid="{00000000-000A-0000-FFFF-FFFF08000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Cheng-Ching Huang" refreshedDate="43087.108064120373" createdVersion="4" refreshedVersion="6" minRefreshableVersion="3" recordCount="271" xr:uid="{00000000-000A-0000-FFFF-FFFF08000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="B3:D274" sheet="工作表1"/>
   </cacheSource>
@@ -1136,16 +1195,19 @@
       <sharedItems containsBlank="1" count="3">
         <s v="p"/>
         <s v="s"/>
-        <m/>
+        <m u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="comments" numFmtId="0">
-      <sharedItems containsBlank="1" count="20">
+      <sharedItems containsBlank="1" count="29">
         <m/>
+        <s v="rstats-db/RSQLite#117"/>
+        <s v="gc() showed 0 warnings"/>
+        <s v="internal error in RS_DBI_getConnection: corrupt connection handle"/>
+        <s v="MySQL server has gone away "/>
+        <s v="target is integer64, current is numeric"/>
+        <s v="Syntax error: 'UNION' is not recognized"/>
         <s v="RMariaDB skips this"/>
-        <s v="target is integer64, current is numeric"/>
-        <s v="MySQL server has gone away "/>
-        <s v="Syntax error: 'UNION' is not recognized"/>
         <s v="Object doesn't exist: function 'date'"/>
         <s v="Unknown column: 'current_date'"/>
         <s v="Object doesn't exist: function 'time'"/>
@@ -1156,11 +1218,17 @@
         <s v="server hang"/>
         <s v="NULL is not supported"/>
         <s v="unlist(unname(rows)) not identical"/>
-        <s v="dbGetQuery(con, &quot;SELECT \&quot;b\&quot; FROM (SELECT 1 AS \&quot;a\&quot;)&quot;) did not throw an error."/>
+        <s v="Objects equal but not identical"/>
         <s v="`actual` not identical to `expected`."/>
         <s v="tweak disabled"/>
         <s v="this test requires supporting NULL value. "/>
         <s v="doesn't support bind"/>
+        <s v="bo returned 0 rows effected"/>
+        <s v="affected shows -1"/>
+        <s v="rstats-db/DBI#55"/>
+        <s v="doesn't support transaction"/>
+        <s v="Cannot allocate a new connection: 16 connections already opened"/>
+        <s v="dbGetQuery(con, &quot;SELECT \&quot;b\&quot; FROM (SELECT 1 AS \&quot;a\&quot;)&quot;) did not throw an error." u="1"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -1173,7 +1241,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="271">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="271">
   <r>
     <s v="package_dependencies"/>
     <x v="0"/>
@@ -1231,8 +1299,8 @@
   </r>
   <r>
     <s v="cannot_forget_disconnect"/>
-    <x v="0"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
   </r>
   <r>
     <s v="disconnect_closed_connection"/>
@@ -1241,8 +1309,8 @@
   </r>
   <r>
     <s v="disconnect_invalid_connection"/>
-    <x v="0"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="data_type_connection"/>
@@ -1261,8 +1329,8 @@
   </r>
   <r>
     <s v="send_query_trivial"/>
-    <x v="1"/>
-    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="send_query_closed_connection"/>
@@ -1271,8 +1339,8 @@
   </r>
   <r>
     <s v="send_query_invalid_connection"/>
-    <x v="0"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="send_query_syntax_error"/>
@@ -1297,144 +1365,144 @@
   <r>
     <s v="send_query_only_one_result_set"/>
     <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <s v="fetch_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="fetch_atomic"/>
+    <x v="1"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="fetch_one_row"/>
+    <x v="1"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="fetch_zero_rows"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="fetch_closed"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="fetch_n_bad"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="fetch_n_good_after_bad"/>
+    <x v="1"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="fetch_no_return_value"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="fetch_multi_row_single_column"/>
+    <x v="1"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="fetch_multi_row_multi_column"/>
+    <x v="1"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="fetch_n_progressive"/>
+    <x v="1"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="fetch_n_multi_row_inf"/>
+    <x v="1"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="fetch_n_more_rows"/>
+    <x v="1"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="fetch_n_zero_rows"/>
+    <x v="1"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="fetch_n_premature_close"/>
+    <x v="1"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="fetch_row_names"/>
+    <x v="1"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="clear_result_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="clear_result_return_query"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="clear_result_return_statement"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="cannot_clear_result_twice_query"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="cannot_clear_result_twice_statement"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_query_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_query_atomic"/>
+    <x v="1"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="get_query_one_row"/>
+    <x v="1"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <s v="get_query_zero_rows"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_query_closed_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_query_invalid_connection"/>
+    <x v="1"/>
     <x v="3"/>
   </r>
   <r>
-    <s v="fetch_formals"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="fetch_atomic"/>
-    <x v="1"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <s v="fetch_one_row"/>
-    <x v="1"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <s v="fetch_zero_rows"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="fetch_closed"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="fetch_n_bad"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="fetch_n_good_after_bad"/>
-    <x v="1"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <s v="fetch_no_return_value"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="fetch_multi_row_single_column"/>
-    <x v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <s v="fetch_multi_row_multi_column"/>
-    <x v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <s v="fetch_n_progressive"/>
-    <x v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <s v="fetch_n_multi_row_inf"/>
-    <x v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <s v="fetch_n_more_rows"/>
-    <x v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <s v="fetch_n_zero_rows"/>
-    <x v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <s v="fetch_n_premature_close"/>
-    <x v="1"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <s v="fetch_row_names"/>
-    <x v="1"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <s v="clear_result_formals"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="clear_result_return_query"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="clear_result_return_statement"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="cannot_clear_result_twice_query"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="cannot_clear_result_twice_statement"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="get_query_formals"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="get_query_atomic"/>
-    <x v="1"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <s v="get_query_one_row"/>
-    <x v="1"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <s v="get_query_zero_rows"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="get_query_closed_connection"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="get_query_invalid_connection"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
     <s v="get_query_syntax_error"/>
     <x v="0"/>
     <x v="0"/>
@@ -1452,42 +1520,42 @@
   <r>
     <s v="get_query_good_after_bad_n"/>
     <x v="1"/>
-    <x v="2"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="get_query_multi_row_single_column"/>
     <x v="1"/>
-    <x v="4"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="get_query_multi_row_multi_column"/>
     <x v="1"/>
-    <x v="4"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="get_query_n_multi_row_inf"/>
     <x v="1"/>
-    <x v="4"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="get_query_n_more_rows"/>
     <x v="1"/>
-    <x v="4"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="get_query_n_zero_rows"/>
     <x v="1"/>
-    <x v="4"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="get_query_n_incomplete"/>
     <x v="1"/>
-    <x v="4"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="get_query_row_names"/>
     <x v="1"/>
-    <x v="2"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="send_statement_formals"/>
@@ -1506,8 +1574,8 @@
   </r>
   <r>
     <s v="send_statement_invalid_connection"/>
-    <x v="0"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="send_statement_syntax_error"/>
@@ -1551,8 +1619,8 @@
   </r>
   <r>
     <s v="execute_invalid_connection"/>
-    <x v="0"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="execute_syntax_error"/>
@@ -1572,1001 +1640,1010 @@
   <r>
     <s v="data_integer"/>
     <x v="1"/>
-    <x v="2"/>
+    <x v="5"/>
   </r>
   <r>
     <s v="data_numeric"/>
     <x v="1"/>
-    <x v="4"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="data_logical"/>
     <x v="1"/>
-    <x v="1"/>
+    <x v="7"/>
   </r>
   <r>
     <s v="data_character"/>
     <x v="1"/>
-    <x v="4"/>
+    <x v="6"/>
   </r>
   <r>
     <s v="data_raw"/>
     <x v="1"/>
-    <x v="1"/>
+    <x v="7"/>
   </r>
   <r>
     <s v="data_date"/>
     <x v="1"/>
-    <x v="5"/>
+    <x v="8"/>
   </r>
   <r>
     <s v="data_date_current"/>
     <x v="1"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <s v="data_time"/>
+    <x v="1"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <s v="data_time_current"/>
+    <x v="1"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <s v="data_timestamp"/>
+    <x v="1"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <s v="data_timestamp_current"/>
+    <x v="1"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <s v="data_null"/>
+    <x v="1"/>
+    <x v="13"/>
+  </r>
+  <r>
+    <s v="data_date_typed"/>
+    <x v="1"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <s v="data_date_current_typed"/>
+    <x v="1"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <s v="data_timestamp_typed"/>
+    <x v="1"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <s v="data_timestamp_current_typed"/>
+    <x v="1"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <s v="data_64_bit_numeric"/>
+    <x v="1"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <s v="data_64_bit_numeric_warning"/>
+    <x v="1"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <s v="data_64_bit_lossless"/>
+    <x v="1"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <s v="quote_string_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="quote_string_return"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="quote_string_vectorized"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="quote_string_double"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="quote_string_roundtrip"/>
+    <x v="1"/>
+    <x v="14"/>
+  </r>
+  <r>
+    <s v="quote_string_na"/>
+    <x v="1"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <s v="quote_string_na_is_null"/>
+    <x v="1"/>
+    <x v="16"/>
+  </r>
+  <r>
+    <s v="quote_identifier_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="quote_identifier_return"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="quote_identifier_vectorized"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="quote_identifier"/>
+    <x v="1"/>
+    <x v="17"/>
+  </r>
+  <r>
+    <s v="quote_identifier_string"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="quote_identifier_special"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_missing"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_empty"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_row_names_false"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_row_names_true_exists"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_row_names_true_missing"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_row_names_na_exists"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_row_names_na_missing"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_row_names_string_exists"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_row_names_string_missing"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_row_names_default"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_check_names"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_closed_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_invalid_connection"/>
+    <x v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="read_table_error"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="read_table_name"/>
+    <x v="1"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <s v="write_table_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="write_table_return"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="write_table_overwrite"/>
+    <x v="1"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <s v="write_table_append_incompatible"/>
+    <x v="1"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <s v="write_table_closed_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="write_table_invalid_connection"/>
+    <x v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="write_table_error"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="write_table_name"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="overwrite_table"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="overwrite_table_missing"/>
+    <x v="1"/>
+    <x v="19"/>
+  </r>
+  <r>
+    <s v="append_table"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="append_table_new"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="temporary_table"/>
+    <x v="0"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <s v="table_visible_in_other_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="roundtrip_keywords"/>
+    <x v="1"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <s v="roundtrip_quotes"/>
+    <x v="1"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <s v="roundtrip_integer"/>
+    <x v="1"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <s v="roundtrip_numeric"/>
+    <x v="1"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <s v="roundtrip_logical"/>
+    <x v="1"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <s v="roundtrip_null"/>
+    <x v="1"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <s v="roundtrip_64_bit_numeric"/>
+    <x v="1"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <s v="roundtrip_64_bit_character"/>
+    <x v="1"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <s v="roundtrip_character"/>
+    <x v="1"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <s v="roundtrip_character_native"/>
+    <x v="1"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <s v="roundtrip_character_empty"/>
+    <x v="1"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <s v="roundtrip_factor"/>
+    <x v="1"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <s v="roundtrip_raw"/>
+    <x v="1"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <s v="roundtrip_blob"/>
+    <x v="1"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <s v="roundtrip_date"/>
+    <x v="1"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <s v="roundtrip_time"/>
+    <x v="1"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <s v="roundtrip_timestamp"/>
+    <x v="1"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <s v="roundtrip_mixed"/>
+    <x v="1"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <s v="roundtrip_field_types"/>
+    <x v="1"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <s v="write_table_row_names_false"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="write_table_row_names_true_exists"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="write_table_row_names_true_missing"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="write_table_row_names_na_exists"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="write_table_row_names_na_missing"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="write_table_row_names_string_exists"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="write_table_row_names_string_missing"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="list_tables_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="list_tables"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="list_tables_closed_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="list_tables_invalid_connection"/>
+    <x v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="exists_table_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="exists_table"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="exists_table_closed_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="exists_table_invalid_connection"/>
+    <x v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="exists_table_error"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="exists_table_name"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="exists_table_list"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="remove_table_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="remove_table_return"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="remove_table_missing"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="remove_table_closed_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="remove_table_invalid_connection"/>
+    <x v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <s v="remove_table_error"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="remove_table_list"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="remove_table_other_con"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="remove_table_temporary"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="remove_table_name"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="list_fields"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="list_fields_row_names"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="bind_formals"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_return_value"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_empty"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_too_many"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_not_enough"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_wrong_name"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_multi_row_unequal_length"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_named_param_unnamed_placeholders"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_named_param_empty_placeholders"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_named_param_na_placeholders"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_unnamed_param_named_placeholders"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_premature_clear"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_multi_row"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_multi_row_zero_length"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_multi_row_statement"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_repeated"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_repeated_untouched"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_integer"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_numeric"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_logical"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_null"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_character"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_factor"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_date"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_timestamp"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_timestamp_lt"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_raw"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="bind_blob"/>
+    <x v="1"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <s v="is_valid_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="is_valid_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="is_valid_stale_connection"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="is_valid_result_query"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="is_valid_result_statement"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="has_completed_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="has_completed_query"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="has_completed_statement"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="has_completed_error"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="has_completed_query_spec"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_statement_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_statement_query"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_statement_statement"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="get_statement_error"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="column_info"/>
+    <x v="1"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <s v="get_row_count_formals"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="row_count_query"/>
+    <x v="1"/>
     <x v="6"/>
   </r>
   <r>
-    <s v="data_time"/>
-    <x v="1"/>
-    <x v="7"/>
-  </r>
-  <r>
-    <s v="data_time_current"/>
-    <x v="1"/>
-    <x v="8"/>
-  </r>
-  <r>
-    <s v="data_timestamp"/>
-    <x v="1"/>
-    <x v="7"/>
-  </r>
-  <r>
-    <s v="data_timestamp_current"/>
-    <x v="1"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <s v="data_null"/>
-    <x v="1"/>
-    <x v="10"/>
-  </r>
-  <r>
-    <s v="data_date_typed"/>
-    <x v="1"/>
-    <x v="5"/>
-  </r>
-  <r>
-    <s v="data_date_current_typed"/>
-    <x v="1"/>
-    <x v="6"/>
-  </r>
-  <r>
-    <s v="data_timestamp_typed"/>
-    <x v="1"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <s v="data_timestamp_current_typed"/>
-    <x v="1"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <s v="data_64_bit_numeric"/>
-    <x v="1"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <s v="data_64_bit_numeric_warning"/>
-    <x v="1"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <s v="data_64_bit_lossless"/>
-    <x v="1"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <s v="quote_string_formals"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="quote_string_return"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="quote_string_vectorized"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="quote_string_double"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="quote_string_roundtrip"/>
-    <x v="1"/>
-    <x v="11"/>
-  </r>
-  <r>
-    <s v="quote_string_na"/>
-    <x v="1"/>
-    <x v="12"/>
-  </r>
-  <r>
-    <s v="quote_string_na_is_null"/>
-    <x v="1"/>
-    <x v="13"/>
-  </r>
-  <r>
-    <s v="quote_identifier_formals"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="quote_identifier_return"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="quote_identifier_vectorized"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="quote_identifier"/>
-    <x v="1"/>
-    <x v="14"/>
-  </r>
-  <r>
-    <s v="quote_identifier_string"/>
-    <x v="1"/>
-    <x v="15"/>
-  </r>
-  <r>
-    <s v="quote_identifier_special"/>
-    <x v="1"/>
-    <x v="14"/>
-  </r>
-  <r>
-    <s v="read_table_formals"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="read_table"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="read_table_missing"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="read_table_empty"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="read_table_row_names_false"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="read_table_row_names_true_exists"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="read_table_row_names_true_missing"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="read_table_row_names_na_exists"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="read_table_row_names_na_missing"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="read_table_row_names_string_exists"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="read_table_row_names_string_missing"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="read_table_row_names_default"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="read_table_check_names"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="read_table_closed_connection"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="read_table_invalid_connection"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="read_table_error"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="read_table_name"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="write_table_formals"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="write_table_return"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="write_table_overwrite"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="write_table_append_incompatible"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="write_table_closed_connection"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="write_table_invalid_connection"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="write_table_error"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="write_table_name"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="overwrite_table"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="overwrite_table_missing"/>
-    <x v="1"/>
-    <x v="16"/>
-  </r>
-  <r>
-    <s v="append_table"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="append_table_new"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="temporary_table"/>
-    <x v="0"/>
-    <x v="17"/>
-  </r>
-  <r>
-    <s v="table_visible_in_other_connection"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="roundtrip_keywords"/>
-    <x v="1"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <s v="roundtrip_quotes"/>
-    <x v="1"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <s v="roundtrip_integer"/>
-    <x v="1"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <s v="roundtrip_numeric"/>
-    <x v="1"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <s v="roundtrip_logical"/>
-    <x v="1"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <s v="roundtrip_null"/>
-    <x v="1"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <s v="roundtrip_64_bit_numeric"/>
-    <x v="1"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <s v="roundtrip_64_bit_character"/>
-    <x v="1"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <s v="roundtrip_character"/>
-    <x v="1"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <s v="roundtrip_character_native"/>
-    <x v="1"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <s v="roundtrip_character_empty"/>
-    <x v="1"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <s v="roundtrip_factor"/>
-    <x v="1"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <s v="roundtrip_raw"/>
-    <x v="1"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <s v="roundtrip_blob"/>
-    <x v="1"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <s v="roundtrip_date"/>
-    <x v="1"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <s v="roundtrip_time"/>
-    <x v="1"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <s v="roundtrip_timestamp"/>
-    <x v="1"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <s v="roundtrip_mixed"/>
-    <x v="1"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <s v="roundtrip_field_types"/>
-    <x v="1"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <s v="write_table_row_names_false"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="write_table_row_names_true_exists"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="write_table_row_names_true_missing"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="write_table_row_names_na_exists"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="write_table_row_names_na_missing"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="write_table_row_names_string_exists"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="write_table_row_names_string_missing"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="list_tables_formals"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="list_tables"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="list_tables_closed_connection"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="list_tables_invalid_connection"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="exists_table_formals"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="exists_table"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="exists_table_closed_connection"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="exists_table_invalid_connection"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="exists_table_error"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="exists_table_name"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="exists_table_list"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="remove_table_formals"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="remove_table_return"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="remove_table_missing"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="remove_table_closed_connection"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="remove_table_invalid_connection"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="remove_table_error"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="remove_table_list"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="remove_table_other_con"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="remove_table_temporary"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="remove_table_name"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="list_fields"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="list_fields_row_names"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="bind_formals"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_return_value"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_empty"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_too_many"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_not_enough"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_wrong_name"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_multi_row_unequal_length"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_named_param_unnamed_placeholders"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_named_param_empty_placeholders"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_named_param_na_placeholders"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_unnamed_param_named_placeholders"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_premature_clear"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_multi_row"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_multi_row_zero_length"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_multi_row_statement"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_repeated"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_repeated_untouched"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_integer"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_numeric"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_logical"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_null"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_character"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_factor"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_date"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_timestamp"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_timestamp_lt"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_raw"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="bind_blob"/>
-    <x v="1"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <s v="is_valid_formals"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="is_valid_connection"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="is_valid_stale_connection"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="is_valid_result_query"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="is_valid_result_statement"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="has_completed_formals"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="has_completed_query"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="has_completed_statement"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="has_completed_error"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="has_completed_query_spec"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="get_statement_formals"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="get_statement_query"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="get_statement_statement"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="get_statement_error"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="column_info"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="get_row_count_formals"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="row_count_query"/>
-    <x v="2"/>
-    <x v="0"/>
-  </r>
-  <r>
     <s v="row_count_statement"/>
-    <x v="2"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <s v="get_row_count_error"/>
-    <x v="2"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <s v="get_rows_affected_formals"/>
-    <x v="2"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <s v="rows_affected_statement"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="23"/>
   </r>
   <r>
     <s v="rows_affected_query"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="24"/>
   </r>
   <r>
     <s v="get_rows_affected_error"/>
-    <x v="2"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <s v="get_info_result"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="25"/>
   </r>
   <r>
     <s v="begin_formals"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="26"/>
   </r>
   <r>
     <s v="commit_formals"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="26"/>
   </r>
   <r>
     <s v="rollback_formals"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="26"/>
   </r>
   <r>
     <s v="begin_commit_return_value"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="26"/>
   </r>
   <r>
     <s v="begin_rollback_return_value"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="26"/>
   </r>
   <r>
     <s v="begin_commit_closed"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="26"/>
   </r>
   <r>
     <s v="begin_commit_invalid"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="26"/>
   </r>
   <r>
     <s v="commit_without_begin"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="26"/>
   </r>
   <r>
     <s v="rollback_without_begin"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="26"/>
   </r>
   <r>
     <s v="begin_begin"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="26"/>
   </r>
   <r>
     <s v="begin_commit"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="26"/>
   </r>
   <r>
     <s v="begin_write_commit"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="26"/>
   </r>
   <r>
     <s v="begin_rollback"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="26"/>
   </r>
   <r>
     <s v="begin_write_rollback"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="26"/>
   </r>
   <r>
     <s v="begin_write_disconnect"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="26"/>
   </r>
   <r>
     <s v="with_transaction_formals"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="26"/>
   </r>
   <r>
     <s v="with_transaction_return_value"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="26"/>
   </r>
   <r>
     <s v="with_transaction_error_closed"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="26"/>
   </r>
   <r>
     <s v="with_transaction_error_invalid"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="26"/>
   </r>
   <r>
     <s v="with_transaction_error_nested"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="26"/>
   </r>
   <r>
     <s v="with_transaction_success"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="26"/>
   </r>
   <r>
     <s v="with_transaction_failure"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="26"/>
   </r>
   <r>
     <s v="with_transaction_break"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="26"/>
   </r>
   <r>
     <s v="with_transaction_side_effects"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="26"/>
   </r>
   <r>
     <s v="compliance"/>
-    <x v="2"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <s v="ellipsis"/>
-    <x v="2"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <s v="simultaneous_connections"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="27"/>
   </r>
   <r>
     <s v="stress_connections"/>
-    <x v="2"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="樞紐分析表1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="數值" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="樞紐分析表1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="數值" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:B30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="4">
         <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
+        <item x="1"/>
+        <item sd="0" m="1" x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisRow" showAll="0">
-      <items count="21">
+      <items count="30">
+        <item m="1" x="28"/>
+        <item x="4"/>
+        <item x="16"/>
+        <item x="8"/>
+        <item x="10"/>
+        <item x="7"/>
         <item x="15"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="9"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="17"/>
+        <item x="14"/>
+        <item x="13"/>
+        <item x="0"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="1"/>
+        <item x="2"/>
         <item x="3"/>
-        <item x="13"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item x="1"/>
-        <item x="12"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="6"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="14"/>
-        <item x="11"/>
-        <item x="10"/>
-        <item x="0"/>
-        <item x="16"/>
-        <item x="17"/>
         <item x="18"/>
-        <item x="19"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2575,15 +2652,90 @@
     <field x="1"/>
     <field x="2"/>
   </rowFields>
-  <rowItems count="4">
+  <rowItems count="29">
     <i>
       <x/>
     </i>
     <i>
       <x v="1"/>
     </i>
-    <i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
       <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="20"/>
+    </i>
+    <i r="1">
+      <x v="21"/>
+    </i>
+    <i r="1">
+      <x v="22"/>
+    </i>
+    <i r="1">
+      <x v="23"/>
+    </i>
+    <i r="1">
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="25"/>
+    </i>
+    <i r="1">
+      <x v="26"/>
+    </i>
+    <i r="1">
+      <x v="27"/>
+    </i>
+    <i r="1">
+      <x v="28"/>
     </i>
     <i t="grand">
       <x/>
@@ -2930,8 +3082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
-      <selection activeCell="C241" sqref="C241"/>
+    <sheetView topLeftCell="A244" workbookViewId="0">
+      <selection activeCell="E271" sqref="E271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3041,7 +3193,7 @@
         <v>288</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>293</v>
+        <v>334</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3095,7 +3247,7 @@
         <v>288</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3117,7 +3269,7 @@
         <v>288</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3139,7 +3291,7 @@
         <v>289</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>293</v>
+        <v>334</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3186,7 +3338,7 @@
         <v>288</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3563,7 +3715,7 @@
         <v>288</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -3731,7 +3883,7 @@
         <v>288</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3823,7 +3975,7 @@
         <v>288</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -4376,7 +4528,7 @@
         <v>288</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -4398,7 +4550,7 @@
         <v>288</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -4430,7 +4582,7 @@
         <v>288</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -4442,7 +4594,7 @@
         <v>288</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -4464,7 +4616,7 @@
         <v>288</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -4506,7 +4658,7 @@
         <v>304</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -4538,7 +4690,7 @@
         <v>309</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -4560,7 +4712,7 @@
         <v>304</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -4572,7 +4724,7 @@
         <v>304</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -4584,7 +4736,7 @@
         <v>304</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -4596,7 +4748,7 @@
         <v>304</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -4608,7 +4760,7 @@
         <v>304</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -4620,7 +4772,7 @@
         <v>304</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -4632,7 +4784,7 @@
         <v>304</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -4644,7 +4796,7 @@
         <v>304</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -4656,7 +4808,7 @@
         <v>304</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -4668,7 +4820,7 @@
         <v>304</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -4680,7 +4832,7 @@
         <v>304</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -4692,7 +4844,7 @@
         <v>304</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -4704,7 +4856,7 @@
         <v>304</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -4716,7 +4868,7 @@
         <v>304</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -4728,7 +4880,7 @@
         <v>304</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4740,7 +4892,7 @@
         <v>304</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4752,7 +4904,7 @@
         <v>304</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4764,7 +4916,7 @@
         <v>304</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -4776,7 +4928,7 @@
         <v>304</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -4888,7 +5040,7 @@
         <v>288</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -4930,7 +5082,7 @@
         <v>288</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -5012,7 +5164,7 @@
         <v>288</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -5071,7 +5223,7 @@
         <v>196</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D193" s="1"/>
     </row>
@@ -5081,7 +5233,7 @@
         <v>197</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D194" s="1"/>
     </row>
@@ -5093,10 +5245,10 @@
         <v>231</v>
       </c>
       <c r="C195" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D195" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D195" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -5105,10 +5257,10 @@
         <v>199</v>
       </c>
       <c r="C196" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D196" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D196" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -5117,10 +5269,10 @@
         <v>200</v>
       </c>
       <c r="C197" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D197" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D197" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -5129,10 +5281,10 @@
         <v>201</v>
       </c>
       <c r="C198" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D198" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D198" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -5141,10 +5293,10 @@
         <v>202</v>
       </c>
       <c r="C199" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D199" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D199" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -5153,10 +5305,10 @@
         <v>203</v>
       </c>
       <c r="C200" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D200" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D200" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -5165,10 +5317,10 @@
         <v>204</v>
       </c>
       <c r="C201" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D201" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D201" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -5177,10 +5329,10 @@
         <v>205</v>
       </c>
       <c r="C202" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D202" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D202" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -5189,10 +5341,10 @@
         <v>206</v>
       </c>
       <c r="C203" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D203" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D203" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -5201,10 +5353,10 @@
         <v>207</v>
       </c>
       <c r="C204" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D204" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D204" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -5213,10 +5365,10 @@
         <v>208</v>
       </c>
       <c r="C205" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D205" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D205" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -5225,10 +5377,10 @@
         <v>209</v>
       </c>
       <c r="C206" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D206" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D206" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -5237,10 +5389,10 @@
         <v>210</v>
       </c>
       <c r="C207" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D207" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D207" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -5249,10 +5401,10 @@
         <v>211</v>
       </c>
       <c r="C208" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D208" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D208" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -5261,10 +5413,10 @@
         <v>212</v>
       </c>
       <c r="C209" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D209" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D209" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -5273,10 +5425,10 @@
         <v>213</v>
       </c>
       <c r="C210" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D210" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D210" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -5285,10 +5437,10 @@
         <v>214</v>
       </c>
       <c r="C211" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D211" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D211" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -5297,10 +5449,10 @@
         <v>215</v>
       </c>
       <c r="C212" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D212" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D212" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5309,10 +5461,10 @@
         <v>216</v>
       </c>
       <c r="C213" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D213" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D213" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -5321,10 +5473,10 @@
         <v>217</v>
       </c>
       <c r="C214" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D214" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D214" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -5333,10 +5485,10 @@
         <v>218</v>
       </c>
       <c r="C215" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D215" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D215" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -5345,10 +5497,10 @@
         <v>219</v>
       </c>
       <c r="C216" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D216" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D216" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -5357,10 +5509,10 @@
         <v>220</v>
       </c>
       <c r="C217" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D217" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D217" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -5369,10 +5521,10 @@
         <v>221</v>
       </c>
       <c r="C218" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D218" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D218" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -5381,10 +5533,10 @@
         <v>222</v>
       </c>
       <c r="C219" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D219" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D219" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -5393,10 +5545,10 @@
         <v>223</v>
       </c>
       <c r="C220" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D220" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D220" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -5405,10 +5557,10 @@
         <v>224</v>
       </c>
       <c r="C221" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D221" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D221" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -5417,10 +5569,10 @@
         <v>225</v>
       </c>
       <c r="C222" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D222" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D222" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -5429,7 +5581,7 @@
         <v>226</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D223" s="1"/>
     </row>
@@ -5439,7 +5591,7 @@
         <v>227</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D224" s="1"/>
     </row>
@@ -5449,7 +5601,7 @@
         <v>228</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D225" s="1"/>
     </row>
@@ -5459,7 +5611,7 @@
         <v>229</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D226" s="1"/>
     </row>
@@ -5468,6 +5620,9 @@
       <c r="B227" s="1" t="s">
         <v>230</v>
       </c>
+      <c r="C227" s="1" t="s">
+        <v>285</v>
+      </c>
       <c r="D227" s="1"/>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -5475,6 +5630,9 @@
       <c r="B228" s="1" t="s">
         <v>232</v>
       </c>
+      <c r="C228" s="1" t="s">
+        <v>285</v>
+      </c>
       <c r="D228" s="1"/>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
@@ -5482,6 +5640,9 @@
       <c r="B229" s="1" t="s">
         <v>233</v>
       </c>
+      <c r="C229" s="1" t="s">
+        <v>285</v>
+      </c>
       <c r="D229" s="1"/>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
@@ -5489,6 +5650,9 @@
       <c r="B230" s="1" t="s">
         <v>234</v>
       </c>
+      <c r="C230" s="1" t="s">
+        <v>285</v>
+      </c>
       <c r="D230" s="1"/>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
@@ -5496,6 +5660,9 @@
       <c r="B231" s="1" t="s">
         <v>235</v>
       </c>
+      <c r="C231" s="1" t="s">
+        <v>285</v>
+      </c>
       <c r="D231" s="1"/>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
@@ -5503,6 +5670,9 @@
       <c r="B232" s="1" t="s">
         <v>236</v>
       </c>
+      <c r="C232" s="1" t="s">
+        <v>285</v>
+      </c>
       <c r="D232" s="1"/>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
@@ -5510,6 +5680,9 @@
       <c r="B233" s="1" t="s">
         <v>237</v>
       </c>
+      <c r="C233" s="1" t="s">
+        <v>285</v>
+      </c>
       <c r="D233" s="1"/>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
@@ -5517,6 +5690,9 @@
       <c r="B234" s="1" t="s">
         <v>238</v>
       </c>
+      <c r="C234" s="1" t="s">
+        <v>285</v>
+      </c>
       <c r="D234" s="1"/>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
@@ -5524,6 +5700,9 @@
       <c r="B235" s="1" t="s">
         <v>239</v>
       </c>
+      <c r="C235" s="1" t="s">
+        <v>285</v>
+      </c>
       <c r="D235" s="1"/>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
@@ -5531,6 +5710,9 @@
       <c r="B236" s="1" t="s">
         <v>240</v>
       </c>
+      <c r="C236" s="1" t="s">
+        <v>285</v>
+      </c>
       <c r="D236" s="1"/>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
@@ -5538,27 +5720,42 @@
       <c r="B237" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="D237" s="1"/>
+      <c r="C237" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D237" s="1" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" s="1"/>
       <c r="B238" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="D238" s="1"/>
+      <c r="C238" s="1" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" s="1"/>
       <c r="B239" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D239" s="1"/>
+      <c r="C239" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D239" s="1" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" s="1"/>
       <c r="B240" s="1" t="s">
         <v>244</v>
       </c>
+      <c r="C240" s="1" t="s">
+        <v>326</v>
+      </c>
       <c r="D240" s="1"/>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -5566,6 +5763,9 @@
       <c r="B241" s="1" t="s">
         <v>245</v>
       </c>
+      <c r="C241" s="1" t="s">
+        <v>326</v>
+      </c>
       <c r="D241" s="1"/>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
@@ -5573,6 +5773,9 @@
       <c r="B242" s="1" t="s">
         <v>246</v>
       </c>
+      <c r="C242" s="1" t="s">
+        <v>326</v>
+      </c>
       <c r="D242" s="1"/>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
@@ -5580,20 +5783,33 @@
       <c r="B243" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="D243" s="1"/>
+      <c r="C243" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D243" s="1" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" s="1"/>
       <c r="B244" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="D244" s="1"/>
+      <c r="C244" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D244" s="1" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" s="1"/>
       <c r="B245" s="1" t="s">
         <v>249</v>
       </c>
+      <c r="C245" s="1" t="s">
+        <v>326</v>
+      </c>
       <c r="D245" s="1"/>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
@@ -5601,7 +5817,12 @@
       <c r="B246" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D246" s="1"/>
+      <c r="C246" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>333</v>
+      </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
@@ -5610,168 +5831,288 @@
       <c r="B247" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="D247" s="1"/>
+      <c r="C247" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" s="1"/>
       <c r="B248" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D248" s="1"/>
+      <c r="C248" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" s="1"/>
       <c r="B249" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="D249" s="1"/>
+      <c r="C249" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D249" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" s="1"/>
       <c r="B250" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="D250" s="1"/>
+      <c r="C250" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D250" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" s="1"/>
       <c r="B251" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="D251" s="1"/>
+      <c r="C251" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D251" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" s="1"/>
       <c r="B252" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D252" s="1"/>
+      <c r="C252" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D252" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" s="1"/>
       <c r="B253" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="D253" s="1"/>
+      <c r="C253" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D253" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" s="1"/>
       <c r="B254" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="D254" s="1"/>
+      <c r="C254" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D254" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" s="1"/>
       <c r="B255" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="D255" s="1"/>
+      <c r="C255" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D255" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" s="1"/>
       <c r="B256" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="D256" s="1"/>
+      <c r="C256" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D256" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" s="1"/>
       <c r="B257" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="D257" s="1"/>
+      <c r="C257" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D257" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" s="1"/>
       <c r="B258" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="D258" s="1"/>
+      <c r="C258" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D258" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" s="1"/>
       <c r="B259" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D259" s="1"/>
+      <c r="C259" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D259" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" s="1"/>
       <c r="B260" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D260" s="1"/>
+      <c r="C260" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D260" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" s="1"/>
       <c r="B261" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="D261" s="1"/>
+      <c r="C261" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D261" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" s="1"/>
       <c r="B262" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="D262" s="1"/>
+      <c r="C262" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D262" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" s="1"/>
       <c r="B263" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="D263" s="1"/>
+      <c r="C263" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D263" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" s="1"/>
       <c r="B264" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="D264" s="1"/>
+      <c r="C264" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D264" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" s="1"/>
       <c r="B265" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="D265" s="1"/>
+      <c r="C265" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D265" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" s="1"/>
       <c r="B266" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="D266" s="1"/>
+      <c r="C266" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D266" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" s="1"/>
       <c r="B267" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="D267" s="1"/>
+      <c r="C267" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D267" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" s="1"/>
       <c r="B268" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="D268" s="1"/>
+      <c r="C268" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D268" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" s="1"/>
       <c r="B269" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D269" s="1"/>
+      <c r="C269" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D269" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" s="1"/>
       <c r="B270" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="D270" s="1"/>
+      <c r="C270" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D270" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
@@ -5779,6 +6120,9 @@
       </c>
       <c r="B271" s="1" t="s">
         <v>277</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>326</v>
       </c>
       <c r="D271" s="1"/>
     </row>
@@ -5787,6 +6131,9 @@
       <c r="B272" s="1" t="s">
         <v>278</v>
       </c>
+      <c r="C272" s="1" t="s">
+        <v>326</v>
+      </c>
       <c r="D272" s="1"/>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
@@ -5796,12 +6143,20 @@
       <c r="B273" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="D273" s="1"/>
+      <c r="C273" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D273" s="1" t="s">
+        <v>343</v>
+      </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" s="1"/>
       <c r="B274" s="1" t="s">
         <v>280</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>326</v>
       </c>
       <c r="D274" s="1"/>
     </row>
@@ -5814,15 +6169,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="1" max="1" width="64" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5831,7 +6186,7 @@
         <v>314</v>
       </c>
       <c r="B1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -5839,7 +6194,7 @@
         <v>308</v>
       </c>
       <c r="B2" s="5">
-        <v>125</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5847,22 +6202,222 @@
         <v>303</v>
       </c>
       <c r="B3" s="5">
-        <v>98</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>316</v>
+      <c r="A4" s="6" t="s">
+        <v>292</v>
       </c>
       <c r="B4" s="5">
-        <v>48</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="B7" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="B8" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="B9" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="B10" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="B11" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="B12" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="B14" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="B17" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="B19" s="5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="B20" s="5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="B21" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="B22" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="B23" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="B24" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="B25" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="B26" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="B27" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="B28" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="B29" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B30" s="5">
         <v>271</v>
       </c>
     </row>

</xml_diff>